<commit_message>
Modify index in new MVC structure
</commit_message>
<xml_diff>
--- a/doc/Journaux_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/doc/Journaux_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub_DATA\I_Shoes_BDD\Documentation\Journaux_de_travail\Romain Lenoir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub_DATA\I_Shoes_BDD\doc\Journaux_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6167A14E-9434-4A12-9C76-671E49DA4102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1F3C18-5F11-4FE9-B38E-7635D4380EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9075" yWindow="1905" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -236,6 +236,12 @@
   <si>
     <t>Change la méthodologie du site pour pouvoir inculquer l'appelation  des views dans le controllers</t>
   </si>
+  <si>
+    <t>Refonte de l'index</t>
+  </si>
+  <si>
+    <t>Modifie l'index en fonction de la nouvelle structure MVC</t>
+  </si>
 </sst>
 </file>
 
@@ -338,7 +344,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -388,12 +394,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1608,7 @@
       <c r="G34" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H34" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1635,74 +1635,142 @@
       <c r="G35" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H35" s="23" t="s">
+      <c r="H35" s="19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>45048</v>
+      </c>
+      <c r="B36" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D36" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="13"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>45050</v>
+      </c>
+      <c r="B37" s="8">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="D37" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="13"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
+        <v>7.6388888888888951E-2</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>45051</v>
+      </c>
+      <c r="B38" s="8">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.66736111111111107</v>
+      </c>
       <c r="D38" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="13"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
+        <v>0.10347222222222219</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>45054</v>
+      </c>
+      <c r="B39" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C39" s="8">
+        <v>0.39861111111111108</v>
+      </c>
       <c r="D39" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
+        <v>6.5277777777777768E-2</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>45056</v>
+      </c>
+      <c r="B40" s="8">
+        <v>0.63750000000000007</v>
+      </c>
+      <c r="C40" s="8">
+        <v>0.70347222222222217</v>
+      </c>
       <c r="D40" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="12"/>
+        <v>6.5972222222222099E-2</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H40" s="20"/>
       <c r="I40" s="13"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>